<commit_message>
Fixed way of SMS app validation in intent
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Intent_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Intent_JS.xlsx
@@ -195,40 +195,6 @@
 </t>
   </si>
   <si>
-    <t>wait(3);
-validate1;
-link_Click(intent_test_link);
-validate2;
-SelectTestToRun(VT200_0430_string);
-ClickRunTest(runtest_top_xpath);
-validate3;
-ClickRunTest(runtest_bottom_xpath);
-wait(5);
-validate4;
-press_Key(Back);
-press_Key(Back);
-ClickUIButtonText(OK);</t>
-  </si>
-  <si>
-    <t>validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Intent JS Test
-};
-validate3
-{
-validate_OldText_Exists=VT200-0430
-};
-validate4
-{
-validate_App_Launched_Device=com.android.mms
-validate_CompareEditText=0,Test_case_passed_if_you_see_this_in_Message_body.
-};</t>
-  </si>
-  <si>
     <t>validate1
 {
 validate_PageTitle=Compliance JS specs
@@ -407,6 +373,32 @@
 wait(5);
 validate4;
 ClickUIButtonText(Close_and_return_result);</t>
+  </si>
+  <si>
+    <t>validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Intent JS Test
+};
+validate3
+{
+validate_OldText_Exists=VT200-0430
+};</t>
+  </si>
+  <si>
+    <t>wait(3);
+validate1;
+link_Click(intent_test_link);
+validate2;
+SelectTestToRun(VT200_0430_string);
+ClickRunTest(runtest_top_xpath);
+validate3;
+ClickRunTest(runtest_bottom_xpath);
+wait(5);
+ExecuteSMSValidation;</t>
   </si>
 </sst>
 </file>
@@ -930,7 +922,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -997,7 +989,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>24</v>
@@ -1022,10 +1014,10 @@
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="H3" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -1045,7 +1037,7 @@
       </c>
       <c r="F4" s="14"/>
       <c r="G4" s="14" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>25</v>
@@ -1079,7 +1071,7 @@
       <c r="J5" s="10"/>
       <c r="K5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="230.25" thickBot="1">
+    <row r="6" spans="1:11" ht="171.75" thickBot="1">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1095,10 +1087,10 @@
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9" t="s">
-        <v>29</v>
+        <v>42</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -1120,7 +1112,7 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>27</v>
@@ -1145,10 +1137,10 @@
       </c>
       <c r="F8" s="9"/>
       <c r="G8" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="10"/>
@@ -1172,10 +1164,10 @@
         <v>1</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
@@ -1198,7 +1190,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>28</v>
@@ -1224,10 +1216,10 @@
         <v>1</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="I11" s="10"/>
       <c r="J11" s="10"/>

</xml_diff>

<commit_message>
Added modified screen shots for Nexus7
</commit_message>
<xml_diff>
--- a/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Intent_JS.xlsx
+++ b/auto/other/UIAutomation/Hybrid_TestNG_Framework/src/com/xls/Intent_JS.xlsx
@@ -258,24 +258,6 @@
 validate5;</t>
   </si>
   <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Intent JS Test
-};
-validate3
-{
-validate_OldText_Exists=VT200-0438
-};
-validate4
-{
-validate_Alert={"data":{"myData":"This is broad cast data 3!"},"appName":"com.rhomobile.compliancetest_js","action":"com.rhomobile.BROADCAST","intentType":"broadcast"}
-</t>
-  </si>
-  <si>
     <t>wait(3);
 validate1;
 link_Click(intent_test_link);
@@ -369,25 +351,6 @@
 ExecuteSMSValidation;</t>
   </si>
   <si>
-    <t xml:space="preserve">validate1
-{
-validate_PageTitle=Compliance JS specs
-};
-validate2
-{
-validate_PageTitle=Intent JS Test
-};
-validate3
-{
-validate_OldText_Exists=VT200-0438
-};
-validate4
-{
-validate_OldText_Exists=VT200-0439
-};
-</t>
-  </si>
-  <si>
     <t>wait(3);
 validate1;
 link_Click(intent_test_link);
@@ -397,14 +360,56 @@
 validate3;
 ClickRunTest(runtest_bottom_xpath);
 wait(2);
+validate4;
+wait(2);
 SelectTestToRun(VT200_0439_string);
 ClickRunTest(runtest_top_xpath);
-validate4;
+validate5;
 ClickRunTest(runtest_bottom_xpath);
 wait(2);
 press_Key(Home);
 launch_App_Device(com.rhomobile.compliancetest_js/com.rhomobile.rhodes.RhodesActivity);
 CheckUITextContains(stoplistening);</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Intent JS Test
+};
+validate3
+{
+validate_OldText_Exists=VT200-0438
+};
+validate4
+{
+validate_Alert={"data":{"myData":"This is broad cast data 3!"},"appName":"com.rhomobile.compliancetest_js","action":"com.rhomobile.BROADCAST","intentType":"broadcast"};
+validate5
+{
+validate_OldText_Exists=VT200-0439
+};
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">validate1
+{
+validate_PageTitle=Compliance JS specs
+};
+validate2
+{
+validate_PageTitle=Intent JS Test
+};
+validate3
+{
+validate_OldText_Exists=VT200-0438
+};
+validate4
+{
+validate_Alert={"data":{"myData":"This is broad cast data 3!"},"appName":"com.rhomobile.compliancetest_js","action":"com.rhomobile.BROADCAST","intentType":"broadcast"};
+</t>
   </si>
 </sst>
 </file>
@@ -928,7 +933,7 @@
   <dimension ref="A1:K11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -995,7 +1000,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="H2" s="9" t="s">
         <v>24</v>
@@ -1020,10 +1025,10 @@
       </c>
       <c r="F3" s="14"/>
       <c r="G3" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="H3" s="14" t="s">
         <v>36</v>
-      </c>
-      <c r="H3" s="14" t="s">
-        <v>37</v>
       </c>
       <c r="I3" s="10"/>
       <c r="J3" s="10"/>
@@ -1093,10 +1098,10 @@
       </c>
       <c r="F6" s="9"/>
       <c r="G6" s="9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H6" s="9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="I6" s="10"/>
       <c r="J6" s="10"/>
@@ -1118,7 +1123,7 @@
       </c>
       <c r="F7" s="9"/>
       <c r="G7" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>27</v>
@@ -1170,16 +1175,16 @@
         <v>1</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="I9" s="10"/>
       <c r="J9" s="10"/>
       <c r="K9" s="2"/>
     </row>
-    <row r="10" spans="1:11" ht="243" thickBot="1">
+    <row r="10" spans="1:11" ht="306.75" thickBot="1">
       <c r="A10" s="12">
         <v>9</v>
       </c>
@@ -1196,7 +1201,7 @@
         <v>1</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>41</v>

</xml_diff>